<commit_message>
mudanco cronograma; artgo para journal e estudo piloto contemplados
</commit_message>
<xml_diff>
--- a/qualificacao/cronograma.xlsx
+++ b/qualificacao/cronograma.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Última disciplina obrigatória</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Mar/2012</t>
+  </si>
+  <si>
+    <t>Escrita de artigo para journal</t>
+  </si>
+  <si>
+    <t>Abr/2012</t>
+  </si>
+  <si>
+    <t>Estudo piloto</t>
   </si>
 </sst>
 </file>
@@ -177,8 +186,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -195,13 +206,15 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -531,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I14"/>
+  <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -550,7 +563,7 @@
     <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" s="6" customFormat="1">
+    <row r="2" spans="1:10" s="6" customFormat="1">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -578,8 +591,11 @@
       <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -591,8 +607,9 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -604,8 +621,9 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -617,8 +635,9 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -630,23 +649,25 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -656,10 +677,11 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -669,62 +691,67 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -733,7 +760,36 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>